<commit_message>
ošetření vstupů a navazující úprava TC
</commit_message>
<xml_diff>
--- a/testovaci scenare.xlsx
+++ b/testovaci scenare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\práce\Python\Engeto\Projekty\Projekt 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B79E10-BC24-4C3A-A9A1-C86CB744E940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7718785-9E1C-4FE1-90A8-E001AB8F3509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="211">
   <si>
     <t>ID</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Reakce na vstup 0</t>
   </si>
   <si>
-    <t>Program vypíše upozornění na nesprávný vstup a znovu zobrazí hlavní nabídku.</t>
-  </si>
-  <si>
     <t>Program vypíše text "Konec programu." a ukončí se.</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
   </si>
   <si>
     <t>Reakce na vstup 5</t>
-  </si>
-  <si>
-    <t>Program zobrazil hlavní nabídku bez upozornění.</t>
   </si>
   <si>
     <t>Přidání úkolu</t>
@@ -233,18 +227,9 @@
     <t>Ověření, že program po zadání vstupu "5" upozorní na nesprávný vstup</t>
   </si>
   <si>
-    <t>Ověření, že program po zadání vstupu "a" upozorní na nesprávný vstup</t>
-  </si>
-  <si>
-    <t>Ověření, že program po zadání vstupu "!" upozorní na nesprávný vstup</t>
-  </si>
-  <si>
     <t>1) Spusťte program main.py
 2) Zadejte vstup "1" a stiskněte Enter
 3) Při výzvě "Zadejte název úkolu:" zadejte prázdný název "" a stiskněte Enter</t>
-  </si>
-  <si>
-    <t>Program vypíše upozornění, že název úkolu nesmí být prázdný a umožní nové zadání názvu.</t>
   </si>
   <si>
     <t>Zadání prázdného popisu úkolu</t>
@@ -262,9 +247,6 @@
 4) Při výzvě "Zadejte popis úkolu:" zadejte prázdný popis "" a stiskněte Enter</t>
   </si>
   <si>
-    <t>Program vypíše upozornění, že popis úkolu nesmí být prázdný a umožní nové zadání popisu.</t>
-  </si>
-  <si>
     <t>Zadání názvu úkolu pouze s mezerami</t>
   </si>
   <si>
@@ -276,34 +258,10 @@
 3) Při výzvě "Zadejte název úkolu:" zadejte název, který sestává z mezer, např. " " a stiskněte Enter</t>
   </si>
   <si>
-    <t>Program vypíše upozornění, že název úkolu musí obsahovat platné znaky a umožní nové zadání názvu.</t>
-  </si>
-  <si>
-    <t>Program vloží úkol s prázdným názvem a pokračuje zobrazením výzvy "Zadejte popis úkolu:"</t>
-  </si>
-  <si>
-    <t>Program vloží prázdný popis úkolu a pokračuje vložením úkolu a zobrazením textu "Úkol 'Úkol 1' byl přidán."</t>
-  </si>
-  <si>
-    <t>Program vloží úkol s názvem, který sestává z mezer a pokračuje zobrazením výzvy "Zadejte popis úkolu:"</t>
-  </si>
-  <si>
     <t>Zadání popisu úkolu pouze s mezerami</t>
   </si>
   <si>
     <t>Ověření, že programu neumožní vložit popisu úkolu pouze s mezerami</t>
-  </si>
-  <si>
-    <t>1) Spusťte program main.py
-2) Zadejte vstup "1" a stiskněte Enter
-3) Při výzvě "Zadejte název úkolu:" zadejte platný název, např. Úkol 1 a stiskněte Enter
-4) Při výzvě "Zadejte popis úkolu:" zadejte popis, který sestává z mezer, např. " " a stiskněte Enter</t>
-  </si>
-  <si>
-    <t>Program vypíše upozornění, že popis úkolu musí obsahovat platné znaky a umožní nové zadání názvu.</t>
-  </si>
-  <si>
-    <t>Program vloží úkol s popisem, který sestává z mezer a pokračuje zobrazením textu "Úkol 'Úkol 1' byl přidán."</t>
   </si>
   <si>
     <t>TC_021</t>
@@ -399,35 +357,11 @@
   </si>
   <si>
     <t>Zobrazení prázdného seznamu</t>
-  </si>
-  <si>
-    <t>Ověření, že program vypisuje prázdný seznam s upozorněním</t>
   </si>
   <si>
     <t>1) Spusťte program main.py
 2) Zadejte vstup "2" a stiskněte Enter
 3) Zkontrolujte, že program zobrazí prázdný seznam</t>
-  </si>
-  <si>
-    <t>Program vypíše text "Seznam úkolů:" a pod ním text "Seznam je prázdný".</t>
-  </si>
-  <si>
-    <t>Program vypíše text "Seznam úkolů:".</t>
-  </si>
-  <si>
-    <t>Zobrazení seznamu s prázdným názvem a popisem úkolu</t>
-  </si>
-  <si>
-    <t>Ověření, že program zobrazí seznam s úkolem, který nemá vyplněný název nebo popis</t>
-  </si>
-  <si>
-    <t>Program zobrazuje hlavní menu a čeká na vstup. Program byl již spuštěn a v proměnné "ukoly" již musí být uložen jeden existující úkol s prázdným jménem a popisem(např. název "", popis "").</t>
-  </si>
-  <si>
-    <t>Program vypíše text "Seznam úkolů:" a pod ním očíslovaný seznam, který obsahuje jednu prázdnou položku "–".</t>
-  </si>
-  <si>
-    <t>Program vypsal text "Seznam úkolů:" a pod ním očíslovaný seznam, který obsahoval jednu prázdnou položku "–".</t>
   </si>
   <si>
     <t>Program vypsal text "Úkol 'Úkol 1' byl odstraněn" a seznam úkolů byl prázdný.</t>
@@ -522,12 +456,6 @@
 3) Zadejte vstup "1" a stiskněte Enter</t>
   </si>
   <si>
-    <t>Program upozorní, že v seznamu úkolů nejsou žádné položky k vymazání a vrátí se do hlavního menu.</t>
-  </si>
-  <si>
-    <t>Program spadne s chybou "IndexError: pop from empty list".</t>
-  </si>
-  <si>
     <t>Odstranění z prázdného seznamu</t>
   </si>
   <si>
@@ -538,12 +466,6 @@
 2) Zadejte vstup "2" a stiskněte Enter</t>
   </si>
   <si>
-    <t>Program upozorní, že se uživatel snaží vymazat neexistující úkol a vrátí se do hlavního menu.</t>
-  </si>
-  <si>
-    <t>Program spadne s chybou "IndexError: pop index out of range"</t>
-  </si>
-  <si>
     <t>Zadání neplatného čísla úkolu při odstraňování</t>
   </si>
   <si>
@@ -575,138 +497,216 @@
 2) Zadejte vstup "" a stiskněte Enter</t>
   </si>
   <si>
-    <t>Program spadne s chybou "ValueError: invalid literal for int() with base 10: ''".</t>
-  </si>
-  <si>
     <t>Ověření, že program při pokusu o zadání vstupu "0" vypíše chybu a nespadne</t>
-  </si>
-  <si>
-    <t>Ověření, že program při pokusu o zadání nečíselného vstupu vypíše chybu a nespadne</t>
   </si>
   <si>
     <t>1) Zadejte vstup "3" a stiskněte Enter
 2) Zadejte vstup "0" a stiskněte Enter</t>
   </si>
   <si>
+    <t>Testuje správné zobrazení hlavního menu, které je klíčové pro navigaci v programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na volbu "1" a správné zavolání funkce pridat_ukol(), která je klíčovou pro fungování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na volbu "2" a správné zavolání funkce zobrazit_ukoly(), která je klíčovou pro fungování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na volbu "3" a správné zavolání funkce odstranit_ukol(), která je klíčovou pro fungování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na volbu "4" a správné ukončení programu, které je klíčovou funkcí programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce pridat_ukol() na zadání prázdného názvu úkolu a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na neplatnou volbu "5" a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na neplatnou volbu "0" a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce pridat_ukol() na zadání názvu úkolu, který sestává z mezer, a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce pridat_ukol() na zadání prázdného popisu úkolu a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce pridat_ukol() na zadání popisu úkolu, který sestává z mezer, a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje, jak funkce zobrazit_ukoly() při vyvolání reaguje, pokud nejsou v proměnné ukoly uložené žádné položky.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce odstranit_ukol() přijme vstup uživatele, odstraní první uložený úkol ze seznamu tří úkolů a vypíše správný text po odstranění.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce odstranit_ukol() přijme vstup uživatele, odstraní poslední uložený úkol ze seznamu tří úkolů a vypíše správný text po odstranění.</t>
+  </si>
+  <si>
+    <t>Testuje, zda se úkoly v seznamu po odstranění jednoho úkolu správně seřadí a nepřeskakují se pořadová čísla, což je důležité pro orientaci v seznamu úkolů.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce odstranit_ukol() na pokus o odstranění úkolu, pokud je seznam prázdný, což je důležité pro správnou funkčnost programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce odstranit_ukol() na pokus o odstranění úkolu při zadání vstupu, který neodpovídá uloženým úkolům, což je důležité pro správnou funkčnost programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na nečíselnou volbu, např. "a", a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci na zadání speciálních znaků, např. "!", a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce odstranit_ukol() při zadání prázdného vstupu a upozornění na neplatný vstup, což je důležité pro správnou funkčnost programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce odstranit_ukol() na neplatný vstup "0" a upozorněn ína neplatný vstup, což je důležité pro správnou funkčnost programu.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce odstranit_ukol() na nečíselný vstup a upozornění na neplatný vstup, což je důležité pro správnou funkčnost programu.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce pridat_ukol() přijme vstup uživatele, přidá nový úkol a vypíše správný text, což je klíčové pro žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce pridat_ukol() přijme vstup uživatele, přidá nový úkol a vypíše správný text při vkládání dalšího úkolu, což je klíčové pro žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce zobrazit_ukoly() po vyvolání korektně zobrazí seznam úkolů přesně s jedním uloženým úkolem, což je klíčové pro žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce zobrazit_ukoly() po vyvolání korektně zobrazí seznam úkolů s více uloženými úkoly, což je klíčové pro žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce odstranit_ukol() přijme vstup uživatele, odstraní jediný uložený úkol a vypíše správný text po odstranění, což je klíčové pro žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Neplatná volba. Zadejte číslo mezi 1 a 4." a umožní novou volbu z nabídky.</t>
+  </si>
+  <si>
+    <t>Program vypsal upozornění "Neplatná volba. Zadejte číslo mezi 1 a 4." a umožnil novou volbu z nabídky.</t>
+  </si>
+  <si>
+    <t>Ověření, že program po zadání písemného vstupu, např. "a", upozorní na nesprávný vstup</t>
+  </si>
+  <si>
+    <t>Ověření, že program po zadání speciálního znaku, např. "!", upozorní na nesprávný vstup</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Název úkolu nesmí být prázdný." a umožní nové zadání názvu.</t>
+  </si>
+  <si>
+    <t>Program vypsal upozornění "Název úkolu nesmí být prázdný." a umožnil nové zadání názvu.</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Popis úkolu nesmí být prázdný." a umožní nové zadání popisu.</t>
+  </si>
+  <si>
+    <t>Program vypsal upozornění "Popis úkolu nesmí být prázdný." a umožnil nové zadání popisu.</t>
+  </si>
+  <si>
+    <t>Ověření, že program upozorní na prázdný seznam</t>
+  </si>
+  <si>
+    <t>Program vypíše text "Seznam úkolů je prázdný".</t>
+  </si>
+  <si>
+    <t>Program vypsal text "Seznam úkolů je prázdný".</t>
+  </si>
+  <si>
+    <t>Duplicitní název úkolu</t>
+  </si>
+  <si>
+    <t>Ověření, že program neumožní zadat stejný název úkolu, který je již uložený v seznamu.</t>
+  </si>
+  <si>
+    <t>1) Zadejte vstup "1" a stiskněte Enter
+3) Při výzvě "Zadejte název úkolu:" zadejte stejný název úkolu jako ten, který je již uložený, např. Úkol 1 a stiskněte Enter
+4) Při výzvě "Zadejte popis úkolu:" zadejte platný popis, např. "Popis k úkolu 1" a stiskněte Enter</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Úkol se stejným názvem již existuje." a umožní nové zadání názvu.</t>
+  </si>
+  <si>
+    <t>Program uložil nový úkol se stejným názvem bez upozornění.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce pridat_ukol() na zadání duplicitního názvu úkolu a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>TC_029</t>
+  </si>
+  <si>
+    <t>Délka názvu úkolu</t>
+  </si>
+  <si>
+    <t>Ověření, že program neumožní zadat příliš dlouhý název úkolu.</t>
+  </si>
+  <si>
+    <t>1) Spusťte program main.py
+2) Zadejte vstup "1" a stiskněte Enter
+3) Při výzvě "Zadejte název úkolu:" zadejte dlouhý název, např. 60x písmeno "a" a stiskněte Enter
+4) Při výzvě "Zadejte popis úkolu:" zadejte platný popis, např. "dlouhý text" a stiskněte Enter</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Název úkolu je omezen na 30 znaků." a umožní nové zadání názvu.</t>
+  </si>
+  <si>
+    <t>Program úkol uložil bez upozornění.</t>
+  </si>
+  <si>
+    <t>Testuje reakci funkce pridat_ukol() na zadání příliš dlouhého názvu úkolu a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění, "Žádné úkoly k odstranění." a vrátí se do hlavního menu.</t>
+  </si>
+  <si>
+    <t>Program vypsal upozornění, "Žádné úkoly k odstranění." a vrátil se do hlavního menu.</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Číslo úkolu musí být 1." a umožní novou volbu.</t>
+  </si>
+  <si>
+    <t>TC_030</t>
+  </si>
+  <si>
+    <t>Zobrazení seznamu před odstraněním</t>
+  </si>
+  <si>
+    <t>Ověření, že program pozadání volby "3" zobrazí seznam uložených úkolů</t>
+  </si>
+  <si>
     <t>1) Zadejte vstup "3" a stiskněte Enter
-2) Zadejte vstup "x" a stiskněte Enter</t>
-  </si>
-  <si>
-    <t>Program upozorní na neplatný vstup a vrátí se do hlavního menu.</t>
-  </si>
-  <si>
-    <t>Program vypsal text "Úkol 'Úkol 1 byl odstraněn." a odstranil Úkol 1 ze seznamu.</t>
-  </si>
-  <si>
-    <t>Program spadne s chybou "ValueError: invalid literal for int() with base 10: 'x'".</t>
-  </si>
-  <si>
-    <t>Testuje správné zobrazení hlavního menu, které je klíčové pro navigaci v programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "1" a správné zavolání funkce pridat_ukol(), která je klíčovou pro chod programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "2" a správné zavolání funkce zobrazit_ukoly(), která je klíčovou pro chod programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "3" a správné zavolání funkce odstranit_ukol(), která je klíčovou pro chod programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "1" a správné ukončení programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na neplatnou volbu "0" a adekvátní vypsání upozornění na nesprávný vstup.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na neplatnou volbu "5" a adekvátní vypsání upozornění na nesprávný vstup.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na neplatnou volbu "a" a adekvátní vypsání upozornění na nesprávný vstup.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na neplatnou volbu "!" a adekvátní vypsání upozornění na nesprávný vstup.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "1" a správné zavolání funkce pridat_ukol(), která je klíčovou pro fungování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "2" a správné zavolání funkce zobrazit_ukoly(), která je klíčovou pro fungování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "3" a správné zavolání funkce odstranit_ukol(), která je klíčovou pro fungování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na volbu "4" a správné ukončení programu, které je klíčovou funkcí programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce pridat_ukol() na zadání prázdného názvu úkolu a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na neplatnou volbu "5" a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na neplatnou volbu "0" a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce pridat_ukol() na zadání názvu úkolu, který sestává z mezer, a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce pridat_ukol() na zadání prázdného popisu úkolu a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce pridat_ukol() na zadání popisu úkolu, který sestává z mezer, a vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje, jak funkce zobrazit_ukoly() při vyvolání reaguje, pokud nejsou v proměnné ukoly uložené žádné položky.</t>
-  </si>
-  <si>
-    <t>Testuje, jak funkce zobrazit_ukoly() při vyvolání reaguje, pokud je v proměnné ukoly uložen úkol, který má prázdný název i popis.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce odstranit_ukol() přijme vstup uživatele, odstraní první uložený úkol ze seznamu tří úkolů a vypíše správný text po odstranění.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce odstranit_ukol() přijme vstup uživatele, odstraní poslední uložený úkol ze seznamu tří úkolů a vypíše správný text po odstranění.</t>
-  </si>
-  <si>
-    <t>Testuje, zda se úkoly v seznamu po odstranění jednoho úkolu správně seřadí a nepřeskakují se pořadová čísla, což je důležité pro orientaci v seznamu úkolů.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce odstranit_ukol() na pokus o odstranění úkolu, pokud je seznam prázdný, což je důležité pro správnou funkčnost programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce odstranit_ukol() na pokus o odstranění úkolu při zadání vstupu, který neodpovídá uloženým úkolům, což je důležité pro správnou funkčnost programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na nečíselnou volbu, např. "a", a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci na zadání speciálních znaků, např. "!", a  vypsání upozornění na nesprávný vstup, který ovlivňuje žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce odstranit_ukol() při zadání prázdného vstupu a upozornění na neplatný vstup, což je důležité pro správnou funkčnost programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce odstranit_ukol() na neplatný vstup "0" a upozorněn ína neplatný vstup, což je důležité pro správnou funkčnost programu.</t>
-  </si>
-  <si>
-    <t>Testuje reakci funkce odstranit_ukol() na nečíselný vstup a upozornění na neplatný vstup, což je důležité pro správnou funkčnost programu.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce pridat_ukol() přijme vstup uživatele, přidá nový úkol a vypíše správný text, což je klíčové pro žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce pridat_ukol() přijme vstup uživatele, přidá nový úkol a vypíše správný text při vkládání dalšího úkolu, což je klíčové pro žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce zobrazit_ukoly() po vyvolání korektně zobrazí seznam úkolů přesně s jedním uloženým úkolem, což je klíčové pro žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce zobrazit_ukoly() po vyvolání korektně zobrazí seznam úkolů s více uloženými úkoly, což je klíčové pro žádané chování programu.</t>
-  </si>
-  <si>
-    <t>Testuje, zda funkce odstranit_ukol() přijme vstup uživatele, odstraní jediný uložený úkol a vypíše správný text po odstranění, což je klíčové pro žádané chování programu.</t>
+2) Zkontrolujte zobrazení seznamu</t>
+  </si>
+  <si>
+    <t>Program vypíše text "Seznam úkolů:" a pod ním očíslovaný seznam, který obsahuje položku "Úkol 1 – Popis k úkolu 1" a níže další text "Zadejte číslo úkolu, který chcete odstranit:".</t>
+  </si>
+  <si>
+    <t>Program vypsal text "Seznam úkolů:" a pod ním očíslovaný seznam, který obsahuje položku "Úkol 1 – Popis k úkolu 1" a níže další text "Zadejte číslo úkolu, který chcete odstranit:".</t>
+  </si>
+  <si>
+    <t>Testuje, zda funkce odstranit_ukol() správně zavolá funkci zobrazit_ukoly(), což je důležité pro správnou funkčnost programu.</t>
+  </si>
+  <si>
+    <t>Program vypíše upozornění "Neplatný vstup. Zadejte číslo úkolu." a umožní novou volbu.</t>
+  </si>
+  <si>
+    <t>Program vypsal upozornění "Neplatný vstup. Zadejte číslo úkolu." a umožnil novou volbu.</t>
+  </si>
+  <si>
+    <t>Program vypsal upozornění "Číslo úkolu musí být 1." a umožnil novou volbu.</t>
+  </si>
+  <si>
+    <t>Ověření, že program při pokusu o zadání nečíselného vstupu, např. "a", vypíše chybu a nespadne</t>
+  </si>
+  <si>
+    <t>1) Zadejte vstup "3" a stiskněte Enter
+2) Zadejte vstup "a" a stiskněte Enter</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,28 +1114,28 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1146,13 +1146,13 @@
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>29</v>
@@ -1164,7 +1164,7 @@
         <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1175,13 +1175,13 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>35</v>
@@ -1193,7 +1193,7 @@
         <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1204,13 +1204,13 @@
         <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>38</v>
@@ -1222,7 +1222,7 @@
         <v>32</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1233,25 +1233,25 @@
         <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1262,25 +1262,25 @@
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1288,28 +1288,28 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1317,28 +1317,28 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1346,28 +1346,28 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -1375,28 +1375,28 @@
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -1404,28 +1404,28 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1433,28 +1433,28 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1462,28 +1462,28 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -1491,434 +1491,489 @@
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>104</v>
+        <v>185</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>111</v>
+        <v>186</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>112</v>
+        <v>187</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>191</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>113</v>
+        <v>193</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>162</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>201</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="1" t="s">
+    </row>
+    <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>206</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>